<commit_message>
Deleted a row from the mental health in tech survey data
</commit_message>
<xml_diff>
--- a/Tech Industry Mental Health Survey.xlsx
+++ b/Tech Industry Mental Health Survey.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\seidu\Documents\GitHub\test_repo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E580E8E1-571D-4428-B469-066847454486}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C271B66-A220-49BE-B263-6FAA257C5500}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -19,7 +19,7 @@
     <sheet name="Meta" sheetId="5" r:id="rId4"/>
   </sheets>
   <definedNames>
-    <definedName name="ExternalData_1" localSheetId="0" hidden="1">survey!$A$1:$AA$1252</definedName>
+    <definedName name="ExternalData_1" localSheetId="0" hidden="1">survey!$A$1:$AA$1251</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -48,7 +48,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30911" uniqueCount="325">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30886" uniqueCount="325">
   <si>
     <t>Date</t>
   </si>
@@ -1194,8 +1194,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{4D9D0778-411A-4140-8486-7FB120170258}" name="survey" displayName="survey" ref="A1:AA1252" tableType="queryTable" totalsRowShown="0">
-  <autoFilter ref="A1:AA1252" xr:uid="{4D9D0778-411A-4140-8486-7FB120170258}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{4D9D0778-411A-4140-8486-7FB120170258}" name="survey" displayName="survey" ref="A1:AA1251" tableType="queryTable" totalsRowShown="0">
+  <autoFilter ref="A1:AA1251" xr:uid="{4D9D0778-411A-4140-8486-7FB120170258}"/>
   <tableColumns count="27">
     <tableColumn id="1" xr3:uid="{BE7B581B-7E51-431B-8A19-CE2234B51847}" uniqueName="1" name="Date" queryTableFieldId="1" dataDxfId="25"/>
     <tableColumn id="2" xr3:uid="{51830EE9-17AF-4292-A35C-FF9E2B5B3A1A}" uniqueName="2" name="Age" queryTableFieldId="2"/>
@@ -1492,10 +1492,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5E9E750F-80D2-48D1-BC5C-FAFB41490975}">
-  <dimension ref="A1:AA1252"/>
+  <dimension ref="A1:AA1251"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="124" zoomScaleNormal="124" workbookViewId="0">
-      <selection activeCell="F18" sqref="F18"/>
+    <sheetView tabSelected="1" topLeftCell="A1228" zoomScale="124" zoomScaleNormal="124" workbookViewId="0">
+      <selection activeCell="I1254" sqref="I1254"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -102863,16 +102863,16 @@
     </row>
     <row r="1238" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A1238" s="1">
-        <v>42129</v>
+        <v>42130</v>
       </c>
       <c r="B1238">
-        <v>32</v>
+        <v>22</v>
       </c>
       <c r="C1238" t="s">
-        <v>12</v>
+        <v>27</v>
       </c>
       <c r="D1238" t="s">
-        <v>30</v>
+        <v>68</v>
       </c>
       <c r="E1238" t="s">
         <v>15</v>
@@ -102881,16 +102881,16 @@
         <v>16</v>
       </c>
       <c r="G1238" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="H1238" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="I1238" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="J1238" t="s">
-        <v>25</v>
+        <v>34</v>
       </c>
       <c r="K1238" t="s">
         <v>16</v>
@@ -102899,19 +102899,19 @@
         <v>16</v>
       </c>
       <c r="M1238" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="N1238" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="O1238" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="P1238" t="s">
-        <v>26</v>
+        <v>17</v>
       </c>
       <c r="Q1238" t="s">
-        <v>26</v>
+        <v>17</v>
       </c>
       <c r="R1238" t="s">
         <v>26</v>
@@ -102920,10 +102920,10 @@
         <v>22</v>
       </c>
       <c r="T1238" t="s">
-        <v>16</v>
+        <v>22</v>
       </c>
       <c r="U1238" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="V1238" t="s">
         <v>17</v>
@@ -102932,16 +102932,16 @@
         <v>16</v>
       </c>
       <c r="X1238" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="Y1238" t="s">
-        <v>16</v>
+        <v>26</v>
       </c>
       <c r="Z1238" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="AA1238" t="s">
-        <v>15</v>
+        <v>279</v>
       </c>
     </row>
     <row r="1239" spans="1:27" x14ac:dyDescent="0.3">
@@ -102949,28 +102949,28 @@
         <v>42130</v>
       </c>
       <c r="B1239">
-        <v>22</v>
+        <v>32</v>
       </c>
       <c r="C1239" t="s">
         <v>27</v>
       </c>
       <c r="D1239" t="s">
-        <v>68</v>
+        <v>13</v>
       </c>
       <c r="E1239" t="s">
-        <v>15</v>
+        <v>72</v>
       </c>
       <c r="F1239" t="s">
         <v>16</v>
       </c>
       <c r="G1239" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="H1239" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="I1239" t="s">
-        <v>18</v>
+        <v>33</v>
       </c>
       <c r="J1239" t="s">
         <v>34</v>
@@ -102979,69 +102979,69 @@
         <v>16</v>
       </c>
       <c r="L1239" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="M1239" t="s">
         <v>17</v>
       </c>
       <c r="N1239" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="O1239" t="s">
-        <v>17</v>
+        <v>26</v>
       </c>
       <c r="P1239" t="s">
         <v>17</v>
       </c>
       <c r="Q1239" t="s">
-        <v>17</v>
+        <v>26</v>
       </c>
       <c r="R1239" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="S1239" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="T1239" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="U1239" t="s">
         <v>16</v>
       </c>
       <c r="V1239" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="W1239" t="s">
-        <v>16</v>
+        <v>22</v>
       </c>
       <c r="X1239" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="Y1239" t="s">
         <v>26</v>
       </c>
       <c r="Z1239" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="AA1239" t="s">
-        <v>279</v>
+        <v>15</v>
       </c>
     </row>
     <row r="1240" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A1240" s="1">
-        <v>42130</v>
+        <v>42131</v>
       </c>
       <c r="B1240">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="C1240" t="s">
         <v>27</v>
       </c>
       <c r="D1240" t="s">
-        <v>13</v>
+        <v>155</v>
       </c>
       <c r="E1240" t="s">
-        <v>72</v>
+        <v>15</v>
       </c>
       <c r="F1240" t="s">
         <v>16</v>
@@ -103050,13 +103050,10 @@
         <v>16</v>
       </c>
       <c r="H1240" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="I1240" t="s">
-        <v>33</v>
-      </c>
-      <c r="J1240" t="s">
-        <v>34</v>
+        <v>18</v>
       </c>
       <c r="K1240" t="s">
         <v>16</v>
@@ -103065,46 +103062,46 @@
         <v>17</v>
       </c>
       <c r="M1240" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="N1240" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="O1240" t="s">
-        <v>26</v>
+        <v>16</v>
       </c>
       <c r="P1240" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="Q1240" t="s">
-        <v>26</v>
+        <v>16</v>
       </c>
       <c r="R1240" t="s">
-        <v>20</v>
+        <v>38</v>
       </c>
       <c r="S1240" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="T1240" t="s">
         <v>16</v>
       </c>
       <c r="U1240" t="s">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="V1240" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="W1240" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="X1240" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="Y1240" t="s">
         <v>26</v>
       </c>
       <c r="Z1240" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="AA1240" t="s">
         <v>15</v>
@@ -103112,31 +103109,34 @@
     </row>
     <row r="1241" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A1241" s="1">
-        <v>42131</v>
+        <v>42180</v>
       </c>
       <c r="B1241">
+        <v>41</v>
+      </c>
+      <c r="C1241" t="s">
+        <v>12</v>
+      </c>
+      <c r="D1241" t="s">
+        <v>13</v>
+      </c>
+      <c r="E1241" t="s">
+        <v>57</v>
+      </c>
+      <c r="F1241" t="s">
+        <v>16</v>
+      </c>
+      <c r="G1241" t="s">
+        <v>17</v>
+      </c>
+      <c r="H1241" t="s">
+        <v>17</v>
+      </c>
+      <c r="I1241" t="s">
         <v>36</v>
       </c>
-      <c r="C1241" t="s">
-        <v>27</v>
-      </c>
-      <c r="D1241" t="s">
-        <v>155</v>
-      </c>
-      <c r="E1241" t="s">
-        <v>15</v>
-      </c>
-      <c r="F1241" t="s">
-        <v>16</v>
-      </c>
-      <c r="G1241" t="s">
-        <v>16</v>
-      </c>
-      <c r="H1241" t="s">
-        <v>17</v>
-      </c>
-      <c r="I1241" t="s">
-        <v>18</v>
+      <c r="J1241" t="s">
+        <v>31</v>
       </c>
       <c r="K1241" t="s">
         <v>16</v>
@@ -103145,7 +103145,7 @@
         <v>17</v>
       </c>
       <c r="M1241" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="N1241" t="s">
         <v>16</v>
@@ -103154,22 +103154,22 @@
         <v>16</v>
       </c>
       <c r="P1241" t="s">
-        <v>16</v>
+        <v>26</v>
       </c>
       <c r="Q1241" t="s">
-        <v>16</v>
+        <v>26</v>
       </c>
       <c r="R1241" t="s">
-        <v>38</v>
+        <v>26</v>
       </c>
       <c r="S1241" t="s">
         <v>17</v>
       </c>
       <c r="T1241" t="s">
-        <v>16</v>
+        <v>22</v>
       </c>
       <c r="U1241" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="V1241" t="s">
         <v>16</v>
@@ -103178,13 +103178,13 @@
         <v>16</v>
       </c>
       <c r="X1241" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="Y1241" t="s">
         <v>26</v>
       </c>
       <c r="Z1241" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="AA1241" t="s">
         <v>15</v>
@@ -103192,19 +103192,19 @@
     </row>
     <row r="1242" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A1242" s="1">
-        <v>42180</v>
+        <v>42207</v>
       </c>
       <c r="B1242">
-        <v>41</v>
+        <v>30</v>
       </c>
       <c r="C1242" t="s">
-        <v>12</v>
+        <v>27</v>
       </c>
       <c r="D1242" t="s">
         <v>13</v>
       </c>
       <c r="E1242" t="s">
-        <v>57</v>
+        <v>41</v>
       </c>
       <c r="F1242" t="s">
         <v>16</v>
@@ -103231,51 +103231,51 @@
         <v>17</v>
       </c>
       <c r="N1242" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="O1242" t="s">
-        <v>16</v>
+        <v>26</v>
       </c>
       <c r="P1242" t="s">
-        <v>26</v>
+        <v>16</v>
       </c>
       <c r="Q1242" t="s">
-        <v>26</v>
+        <v>17</v>
       </c>
       <c r="R1242" t="s">
-        <v>26</v>
+        <v>46</v>
       </c>
       <c r="S1242" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="T1242" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="U1242" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="V1242" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="W1242" t="s">
-        <v>16</v>
+        <v>22</v>
       </c>
       <c r="X1242" t="s">
-        <v>16</v>
+        <v>22</v>
       </c>
       <c r="Y1242" t="s">
-        <v>26</v>
+        <v>17</v>
       </c>
       <c r="Z1242" t="s">
         <v>16</v>
       </c>
       <c r="AA1242" t="s">
-        <v>15</v>
+        <v>280</v>
       </c>
     </row>
     <row r="1243" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A1243" s="1">
-        <v>42207</v>
+        <v>42212</v>
       </c>
       <c r="B1243">
         <v>30</v>
@@ -103290,7 +103290,7 @@
         <v>41</v>
       </c>
       <c r="F1243" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="G1243" t="s">
         <v>17</v>
@@ -103299,7 +103299,7 @@
         <v>17</v>
       </c>
       <c r="I1243" t="s">
-        <v>36</v>
+        <v>18</v>
       </c>
       <c r="J1243" t="s">
         <v>31</v>
@@ -103314,19 +103314,19 @@
         <v>17</v>
       </c>
       <c r="N1243" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="O1243" t="s">
-        <v>26</v>
+        <v>17</v>
       </c>
       <c r="P1243" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="Q1243" t="s">
-        <v>17</v>
+        <v>26</v>
       </c>
       <c r="R1243" t="s">
-        <v>46</v>
+        <v>26</v>
       </c>
       <c r="S1243" t="s">
         <v>16</v>
@@ -103335,7 +103335,7 @@
         <v>16</v>
       </c>
       <c r="U1243" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="V1243" t="s">
         <v>17</v>
@@ -103353,27 +103353,27 @@
         <v>16</v>
       </c>
       <c r="AA1243" t="s">
-        <v>280</v>
+        <v>15</v>
       </c>
     </row>
     <row r="1244" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A1244" s="1">
-        <v>42212</v>
+        <v>42233</v>
       </c>
       <c r="B1244">
-        <v>30</v>
+        <v>36</v>
       </c>
       <c r="C1244" t="s">
         <v>27</v>
       </c>
       <c r="D1244" t="s">
-        <v>13</v>
+        <v>105</v>
       </c>
       <c r="E1244" t="s">
-        <v>41</v>
+        <v>15</v>
       </c>
       <c r="F1244" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G1244" t="s">
         <v>17</v>
@@ -103385,31 +103385,31 @@
         <v>18</v>
       </c>
       <c r="J1244" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="K1244" t="s">
         <v>16</v>
       </c>
       <c r="L1244" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="M1244" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="N1244" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="O1244" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="P1244" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="Q1244" t="s">
         <v>26</v>
       </c>
       <c r="R1244" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="S1244" t="s">
         <v>16</v>
@@ -103424,10 +103424,10 @@
         <v>17</v>
       </c>
       <c r="W1244" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="X1244" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="Y1244" t="s">
         <v>17</v>
@@ -103441,61 +103441,61 @@
     </row>
     <row r="1245" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A1245" s="1">
-        <v>42233</v>
+        <v>42236</v>
       </c>
       <c r="B1245">
+        <v>29</v>
+      </c>
+      <c r="C1245" t="s">
+        <v>27</v>
+      </c>
+      <c r="D1245" t="s">
+        <v>13</v>
+      </c>
+      <c r="E1245" t="s">
+        <v>51</v>
+      </c>
+      <c r="F1245" t="s">
+        <v>16</v>
+      </c>
+      <c r="G1245" t="s">
+        <v>17</v>
+      </c>
+      <c r="H1245" t="s">
+        <v>17</v>
+      </c>
+      <c r="I1245" t="s">
         <v>36</v>
-      </c>
-      <c r="C1245" t="s">
-        <v>27</v>
-      </c>
-      <c r="D1245" t="s">
-        <v>105</v>
-      </c>
-      <c r="E1245" t="s">
-        <v>15</v>
-      </c>
-      <c r="F1245" t="s">
-        <v>16</v>
-      </c>
-      <c r="G1245" t="s">
-        <v>17</v>
-      </c>
-      <c r="H1245" t="s">
-        <v>17</v>
-      </c>
-      <c r="I1245" t="s">
-        <v>18</v>
       </c>
       <c r="J1245" t="s">
         <v>34</v>
       </c>
       <c r="K1245" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="L1245" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="M1245" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="N1245" t="s">
         <v>17</v>
       </c>
       <c r="O1245" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="P1245" t="s">
         <v>16</v>
       </c>
       <c r="Q1245" t="s">
-        <v>26</v>
+        <v>17</v>
       </c>
       <c r="R1245" t="s">
-        <v>20</v>
+        <v>26</v>
       </c>
       <c r="S1245" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="T1245" t="s">
         <v>16</v>
@@ -103504,16 +103504,16 @@
         <v>21</v>
       </c>
       <c r="V1245" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="W1245" t="s">
         <v>16</v>
       </c>
       <c r="X1245" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="Y1245" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="Z1245" t="s">
         <v>16</v>
@@ -103524,10 +103524,10 @@
     </row>
     <row r="1246" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A1246" s="1">
-        <v>42236</v>
+        <v>42241</v>
       </c>
       <c r="B1246">
-        <v>29</v>
+        <v>36</v>
       </c>
       <c r="C1246" t="s">
         <v>27</v>
@@ -103536,7 +103536,7 @@
         <v>13</v>
       </c>
       <c r="E1246" t="s">
-        <v>51</v>
+        <v>64</v>
       </c>
       <c r="F1246" t="s">
         <v>16</v>
@@ -103545,58 +103545,58 @@
         <v>17</v>
       </c>
       <c r="H1246" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="I1246" t="s">
-        <v>36</v>
+        <v>24</v>
       </c>
       <c r="J1246" t="s">
-        <v>34</v>
+        <v>25</v>
       </c>
       <c r="K1246" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="L1246" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="M1246" t="s">
-        <v>17</v>
+        <v>26</v>
       </c>
       <c r="N1246" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="O1246" t="s">
         <v>17</v>
       </c>
       <c r="P1246" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="Q1246" t="s">
-        <v>17</v>
+        <v>26</v>
       </c>
       <c r="R1246" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="S1246" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="T1246" t="s">
-        <v>16</v>
+        <v>22</v>
       </c>
       <c r="U1246" t="s">
         <v>21</v>
       </c>
       <c r="V1246" t="s">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="W1246" t="s">
         <v>16</v>
       </c>
       <c r="X1246" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="Y1246" t="s">
-        <v>16</v>
+        <v>26</v>
       </c>
       <c r="Z1246" t="s">
         <v>16</v>
@@ -103607,52 +103607,52 @@
     </row>
     <row r="1247" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A1247" s="1">
-        <v>42241</v>
+        <v>42259</v>
       </c>
       <c r="B1247">
-        <v>36</v>
+        <v>26</v>
       </c>
       <c r="C1247" t="s">
         <v>27</v>
       </c>
       <c r="D1247" t="s">
-        <v>13</v>
+        <v>30</v>
       </c>
       <c r="E1247" t="s">
-        <v>64</v>
+        <v>15</v>
       </c>
       <c r="F1247" t="s">
         <v>16</v>
       </c>
       <c r="G1247" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="H1247" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="I1247" t="s">
-        <v>24</v>
+        <v>15</v>
       </c>
       <c r="J1247" t="s">
-        <v>25</v>
+        <v>31</v>
       </c>
       <c r="K1247" t="s">
         <v>16</v>
       </c>
       <c r="L1247" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="M1247" t="s">
-        <v>26</v>
+        <v>16</v>
       </c>
       <c r="N1247" t="s">
         <v>16</v>
       </c>
       <c r="O1247" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="P1247" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="Q1247" t="s">
         <v>26</v>
@@ -103661,10 +103661,10 @@
         <v>20</v>
       </c>
       <c r="S1247" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="T1247" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="U1247" t="s">
         <v>21</v>
@@ -103690,46 +103690,46 @@
     </row>
     <row r="1248" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A1248" s="1">
-        <v>42259</v>
+        <v>42273</v>
       </c>
       <c r="B1248">
-        <v>26</v>
+        <v>32</v>
       </c>
       <c r="C1248" t="s">
         <v>27</v>
       </c>
       <c r="D1248" t="s">
-        <v>30</v>
+        <v>13</v>
       </c>
       <c r="E1248" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F1248" t="s">
         <v>16</v>
       </c>
       <c r="G1248" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="H1248" t="s">
         <v>17</v>
       </c>
       <c r="I1248" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="J1248" t="s">
         <v>31</v>
       </c>
       <c r="K1248" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="L1248" t="s">
         <v>17</v>
       </c>
       <c r="M1248" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="N1248" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="O1248" t="s">
         <v>16</v>
@@ -103738,10 +103738,10 @@
         <v>16</v>
       </c>
       <c r="Q1248" t="s">
-        <v>26</v>
+        <v>17</v>
       </c>
       <c r="R1248" t="s">
-        <v>20</v>
+        <v>29</v>
       </c>
       <c r="S1248" t="s">
         <v>16</v>
@@ -103753,7 +103753,7 @@
         <v>21</v>
       </c>
       <c r="V1248" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="W1248" t="s">
         <v>16</v>
@@ -103762,7 +103762,7 @@
         <v>16</v>
       </c>
       <c r="Y1248" t="s">
-        <v>26</v>
+        <v>17</v>
       </c>
       <c r="Z1248" t="s">
         <v>16</v>
@@ -103773,10 +103773,10 @@
     </row>
     <row r="1249" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A1249" s="1">
-        <v>42273</v>
+        <v>42315</v>
       </c>
       <c r="B1249">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="C1249" t="s">
         <v>27</v>
@@ -103785,7 +103785,7 @@
         <v>13</v>
       </c>
       <c r="E1249" t="s">
-        <v>14</v>
+        <v>41</v>
       </c>
       <c r="F1249" t="s">
         <v>16</v>
@@ -103797,13 +103797,13 @@
         <v>17</v>
       </c>
       <c r="I1249" t="s">
-        <v>18</v>
+        <v>36</v>
       </c>
       <c r="J1249" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="K1249" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="L1249" t="s">
         <v>17</v>
@@ -103821,22 +103821,22 @@
         <v>16</v>
       </c>
       <c r="Q1249" t="s">
-        <v>17</v>
+        <v>26</v>
       </c>
       <c r="R1249" t="s">
         <v>29</v>
       </c>
       <c r="S1249" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="T1249" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="U1249" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="V1249" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="W1249" t="s">
         <v>16</v>
@@ -103845,7 +103845,7 @@
         <v>16</v>
       </c>
       <c r="Y1249" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="Z1249" t="s">
         <v>16</v>
@@ -103856,43 +103856,43 @@
     </row>
     <row r="1250" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A1250" s="1">
-        <v>42315</v>
+        <v>42338</v>
       </c>
       <c r="B1250">
-        <v>34</v>
+        <v>46</v>
       </c>
       <c r="C1250" t="s">
-        <v>27</v>
+        <v>12</v>
       </c>
       <c r="D1250" t="s">
         <v>13</v>
       </c>
       <c r="E1250" t="s">
-        <v>41</v>
+        <v>51</v>
       </c>
       <c r="F1250" t="s">
         <v>16</v>
       </c>
       <c r="G1250" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="H1250" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="I1250" t="s">
-        <v>36</v>
+        <v>15</v>
       </c>
       <c r="J1250" t="s">
-        <v>25</v>
+        <v>34</v>
       </c>
       <c r="K1250" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="L1250" t="s">
         <v>17</v>
       </c>
       <c r="M1250" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="N1250" t="s">
         <v>17</v>
@@ -103907,13 +103907,13 @@
         <v>26</v>
       </c>
       <c r="R1250" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="S1250" t="s">
         <v>17</v>
       </c>
       <c r="T1250" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="U1250" t="s">
         <v>16</v>
@@ -103939,43 +103939,43 @@
     </row>
     <row r="1251" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A1251" s="1">
-        <v>42338</v>
+        <v>42401</v>
       </c>
       <c r="B1251">
-        <v>46</v>
+        <v>25</v>
       </c>
       <c r="C1251" t="s">
-        <v>12</v>
+        <v>27</v>
       </c>
       <c r="D1251" t="s">
         <v>13</v>
       </c>
       <c r="E1251" t="s">
-        <v>51</v>
+        <v>14</v>
       </c>
       <c r="F1251" t="s">
         <v>16</v>
       </c>
       <c r="G1251" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="H1251" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="I1251" t="s">
-        <v>15</v>
+        <v>36</v>
       </c>
       <c r="J1251" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="K1251" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="L1251" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="M1251" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="N1251" t="s">
         <v>17</v>
@@ -103987,19 +103987,19 @@
         <v>16</v>
       </c>
       <c r="Q1251" t="s">
-        <v>26</v>
+        <v>17</v>
       </c>
       <c r="R1251" t="s">
         <v>26</v>
       </c>
       <c r="S1251" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="T1251" t="s">
         <v>16</v>
       </c>
       <c r="U1251" t="s">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="V1251" t="s">
         <v>16</v>
@@ -104011,95 +104011,12 @@
         <v>16</v>
       </c>
       <c r="Y1251" t="s">
-        <v>16</v>
+        <v>26</v>
       </c>
       <c r="Z1251" t="s">
         <v>16</v>
       </c>
       <c r="AA1251" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="1252" spans="1:27" x14ac:dyDescent="0.3">
-      <c r="A1252" s="1">
-        <v>42401</v>
-      </c>
-      <c r="B1252">
-        <v>25</v>
-      </c>
-      <c r="C1252" t="s">
-        <v>27</v>
-      </c>
-      <c r="D1252" t="s">
-        <v>13</v>
-      </c>
-      <c r="E1252" t="s">
-        <v>14</v>
-      </c>
-      <c r="F1252" t="s">
-        <v>16</v>
-      </c>
-      <c r="G1252" t="s">
-        <v>17</v>
-      </c>
-      <c r="H1252" t="s">
-        <v>17</v>
-      </c>
-      <c r="I1252" t="s">
-        <v>36</v>
-      </c>
-      <c r="J1252" t="s">
-        <v>31</v>
-      </c>
-      <c r="K1252" t="s">
-        <v>16</v>
-      </c>
-      <c r="L1252" t="s">
-        <v>16</v>
-      </c>
-      <c r="M1252" t="s">
-        <v>17</v>
-      </c>
-      <c r="N1252" t="s">
-        <v>17</v>
-      </c>
-      <c r="O1252" t="s">
-        <v>16</v>
-      </c>
-      <c r="P1252" t="s">
-        <v>16</v>
-      </c>
-      <c r="Q1252" t="s">
-        <v>17</v>
-      </c>
-      <c r="R1252" t="s">
-        <v>26</v>
-      </c>
-      <c r="S1252" t="s">
-        <v>22</v>
-      </c>
-      <c r="T1252" t="s">
-        <v>16</v>
-      </c>
-      <c r="U1252" t="s">
-        <v>21</v>
-      </c>
-      <c r="V1252" t="s">
-        <v>16</v>
-      </c>
-      <c r="W1252" t="s">
-        <v>16</v>
-      </c>
-      <c r="X1252" t="s">
-        <v>16</v>
-      </c>
-      <c r="Y1252" t="s">
-        <v>26</v>
-      </c>
-      <c r="Z1252" t="s">
-        <v>16</v>
-      </c>
-      <c r="AA1252" t="s">
         <v>15</v>
       </c>
     </row>

</xml_diff>